<commit_message>
-Update dntt đặt xe, sửa form tổng hợp cá nhân, update thêm trường cho chức năng sửa chữa xe
</commit_message>
<xml_diff>
--- a/public/assets/templateForm/MauTheoDoiXe.xlsx
+++ b/public/assets/templateForm/MauTheoDoiXe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lung Dep Trai\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RTC\R_ERPWeb\Frontend\RERP_FRONTEND_V2\RERP_FRONTEND_V2\public\assets\templateForm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7259FD6-4973-4373-BB0D-87A455A98C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1EC3D7-EA1D-40EE-8A2A-41118A082B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="630" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Triton" sheetId="4" state="hidden" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="123">
   <si>
     <t>STT</t>
   </si>
@@ -459,6 +459,15 @@
   </si>
   <si>
     <t>THEO DÕI BẢO DƯỠNG, SỬA CHỮA, THAY THẾ THIẾT BỊ XE XXX</t>
+  </si>
+  <si>
+    <t>Số KM kỳ trước</t>
+  </si>
+  <si>
+    <t>Số KM kỳ này</t>
+  </si>
+  <si>
+    <t>Số KM trong kỳ</t>
   </si>
 </sst>
 </file>
@@ -2021,7 +2030,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="60">
+    <row r="12" spans="1:17" ht="75">
       <c r="A12" s="10">
         <v>8</v>
       </c>
@@ -2062,7 +2071,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="60">
+    <row r="13" spans="1:17" ht="75">
       <c r="A13" s="10">
         <v>9</v>
       </c>
@@ -8492,10 +8501,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA21DB5-DE42-4680-B48A-E6C4D7532729}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8505,19 +8514,19 @@
     <col min="3" max="3" width="28.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="6" width="25.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="13" width="28" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" customWidth="1"/>
-    <col min="17" max="17" width="52" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="28" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" customWidth="1"/>
+    <col min="19" max="19" width="18.42578125" customWidth="1"/>
+    <col min="20" max="20" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="30.6" customHeight="1">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="30.6" customHeight="1">
       <c r="A1" s="53" t="s">
         <v>119</v>
       </c>
@@ -8537,8 +8546,11 @@
       <c r="O1" s="53"/>
       <c r="P1" s="53"/>
       <c r="Q1" s="53"/>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" ht="15.6" customHeight="1">
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+    </row>
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="15.6" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -8550,14 +8562,17 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
       <c r="O2" s="15"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" ht="15.6" customHeight="1">
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" s="1" customFormat="1" ht="15.6" customHeight="1">
       <c r="A3" s="54" t="s">
         <v>18</v>
       </c>
@@ -8574,17 +8589,20 @@
       <c r="J3" s="58"/>
       <c r="K3" s="58"/>
       <c r="L3" s="58"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="60" t="s">
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="61" t="s">
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="61" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" ht="63">
+    <row r="4" spans="1:20" s="1" customFormat="1" ht="63">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -8604,44 +8622,53 @@
         <v>26</v>
       </c>
       <c r="G4" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="O4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="P4" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="Q4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="R4" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="S4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="61"/>
+      <c r="T4" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A1:T1"/>
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="G3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="T3:T4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
mau theo doi xe
</commit_message>
<xml_diff>
--- a/public/assets/templateForm/MauTheoDoiXe.xlsx
+++ b/public/assets/templateForm/MauTheoDoiXe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RTC\R_ERPWeb\Frontend\RERP_FRONTEND_V2\RERP_FRONTEND_V2\public\assets\templateForm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1EC3D7-EA1D-40EE-8A2A-41118A082B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89477EC0-C3B6-4B9C-B461-D29D1F29146B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28350" yWindow="750" windowWidth="21600" windowHeight="12645" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Triton" sheetId="4" state="hidden" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="124">
   <si>
     <t>STT</t>
   </si>
@@ -468,6 +468,9 @@
   </si>
   <si>
     <t>Số KM trong kỳ</t>
+  </si>
+  <si>
+    <t>Ngày kỳ trước</t>
   </si>
 </sst>
 </file>
@@ -551,7 +554,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -591,6 +594,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -719,7 +728,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -900,6 +909,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1950,7 +1962,7 @@
       <c r="P9" s="10"/>
       <c r="Q9" s="22"/>
     </row>
-    <row r="10" spans="1:17" ht="75">
+    <row r="10" spans="1:17" ht="60">
       <c r="A10" s="10">
         <v>6</v>
       </c>
@@ -1989,7 +2001,7 @@
       <c r="P10" s="10"/>
       <c r="Q10" s="22"/>
     </row>
-    <row r="11" spans="1:17" ht="90">
+    <row r="11" spans="1:17" ht="75">
       <c r="A11" s="10">
         <v>7</v>
       </c>
@@ -2030,7 +2042,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="75">
+    <row r="12" spans="1:17" ht="60">
       <c r="A12" s="10">
         <v>8</v>
       </c>
@@ -2071,7 +2083,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="75">
+    <row r="13" spans="1:17" ht="60">
       <c r="A13" s="10">
         <v>9</v>
       </c>
@@ -8501,10 +8513,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA21DB5-DE42-4680-B48A-E6C4D7532729}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8514,19 +8526,20 @@
     <col min="3" max="3" width="28.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="6" width="25.28515625" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" customWidth="1"/>
-    <col min="16" max="16" width="28" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" customWidth="1"/>
-    <col min="18" max="18" width="18.140625" customWidth="1"/>
-    <col min="19" max="19" width="18.42578125" customWidth="1"/>
-    <col min="20" max="20" width="52" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="28" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" customWidth="1"/>
+    <col min="19" max="19" width="18.140625" customWidth="1"/>
+    <col min="20" max="20" width="18.42578125" customWidth="1"/>
+    <col min="21" max="21" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="30.6" customHeight="1">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="30.6" customHeight="1">
       <c r="A1" s="53" t="s">
         <v>119</v>
       </c>
@@ -8549,8 +8562,9 @@
       <c r="R1" s="53"/>
       <c r="S1" s="53"/>
       <c r="T1" s="53"/>
-    </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="15.6" customHeight="1">
+      <c r="U1" s="53"/>
+    </row>
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="15.6" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -8565,14 +8579,15 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="15"/>
+      <c r="O2" s="4"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
-      <c r="S2" s="4"/>
+      <c r="S2" s="15"/>
       <c r="T2" s="4"/>
-    </row>
-    <row r="3" spans="1:20" s="1" customFormat="1" ht="15.6" customHeight="1">
+      <c r="U2" s="4"/>
+    </row>
+    <row r="3" spans="1:21" s="1" customFormat="1" ht="15.6" customHeight="1">
       <c r="A3" s="54" t="s">
         <v>18</v>
       </c>
@@ -8592,17 +8607,18 @@
       <c r="M3" s="58"/>
       <c r="N3" s="58"/>
       <c r="O3" s="58"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="60" t="s">
+      <c r="P3" s="58"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="60"/>
       <c r="S3" s="60"/>
-      <c r="T3" s="61" t="s">
+      <c r="T3" s="60"/>
+      <c r="U3" s="61" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="1" customFormat="1" ht="63">
+    <row r="4" spans="1:21" s="1" customFormat="1" ht="63">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -8621,54 +8637,57 @@
       <c r="F4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="62" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="P4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="P4" s="17" t="s">
+      <c r="Q4" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="Q4" s="16" t="s">
+      <c r="R4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="16" t="s">
+      <c r="S4" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="S4" s="16" t="s">
+      <c r="T4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="T4" s="61"/>
+      <c r="U4" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A1:U1"/>
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="G3:Q3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>